<commit_message>
collected all click worker responses
</commit_message>
<xml_diff>
--- a/07-Amazon_MTurk_click_worker_response_30cow_pairwise/results/click_worker_HIT_submit_track.xlsx
+++ b/07-Amazon_MTurk_click_worker_response_30cow_pairwise/results/click_worker_HIT_submit_track.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/University of British Columbia/Research/PhD Project/Amazon project phase 2/Sora Jeong/results/Amazon MTurk click worker response/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/07-Amazon_MTurk_click_worker_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{EEC6DB9E-F389-F641-9099-D0AB0447A80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2413C57-A2DB-EB43-9421-49FDC037E6E0}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{EEC6DB9E-F389-F641-9099-D0AB0447A80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6EF4B3-51BF-0941-AD72-10EEAB493133}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{BB8A2956-08A4-8344-AB72-98E0316C1697}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BB8A2956-08A4-8344-AB72-98E0316C1697}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>master_all_responses_click_worker_Sep-13-2023.csv</t>
   </si>
   <si>
-    <t>not complete: master_all_responses_click_worker_44HITsSep-13-2023.csv</t>
+    <t>master_all_responses_click_worker_44HITsOct-01-2023.csv</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +490,7 @@
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>